<commit_message>
5. Best 5 v1.1
Add other Columns
</commit_message>
<xml_diff>
--- a/results/double_strollers_All.xlsx
+++ b/results/double_strollers_All.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deank\Passive_Income\Best_Reviews__Blog\Scraper\Google_Shopping_Scraper\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866AB192-2319-4BE8-8DE4-9D041CECD8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E36421-B2B0-4E3D-8D33-60C0C4E9505A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="37900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2120" yWindow="2680" windowWidth="16200" windowHeight="27970" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5671" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5930" uniqueCount="693">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -27053,14 +27053,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.36328125" customWidth="1"/>
     <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="27.08984375" customWidth="1"/>
+    <col min="9" max="9" width="23.7265625" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -27088,25 +27091,25 @@
       <c r="H1" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>366</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>369</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>686</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>687</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>688</v>
       </c>
       <c r="P1" s="3" t="s">
@@ -32990,25 +32993,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.54296875" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" customWidth="1"/>
-    <col min="5" max="5" width="20.1796875" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="11.90625" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>489</v>
       </c>
@@ -33036,37 +33032,64 @@
       <c r="I1" s="4" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>310</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>311</v>
+        <v>113</v>
       </c>
       <c r="C2">
-        <v>4.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D2">
-        <v>627</v>
+        <v>6450</v>
       </c>
       <c r="E2">
-        <v>4.5579999999999998</v>
+        <v>4.2290000000000001</v>
       </c>
       <c r="F2">
-        <v>0.8571428571428571</v>
+        <v>0.68421052631578949</v>
       </c>
       <c r="G2">
-        <v>6.4425401664681976</v>
+        <v>8.7719904365322421</v>
       </c>
       <c r="H2">
-        <v>4.2857142857142856</v>
+        <v>3.4210526315789469</v>
       </c>
       <c r="I2">
-        <v>4.3689873612815404</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>4.41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>372</v>
+      </c>
+      <c r="K2">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="L2" t="s">
+        <v>384</v>
+      </c>
+      <c r="N2">
+        <v>4.82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -33092,94 +33115,2601 @@
         <v>3.4210526315789469</v>
       </c>
       <c r="I3">
-        <v>4.3329105263157892</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>4.41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>387</v>
+      </c>
+      <c r="K3">
+        <v>21.2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>437</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>329</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>113</v>
       </c>
       <c r="C4">
         <v>4.5999999999999996</v>
       </c>
       <c r="D4">
-        <v>380</v>
+        <v>6450</v>
       </c>
       <c r="E4">
-        <v>4.2122222222222216</v>
+        <v>4.2290000000000001</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0.68421052631578949</v>
       </c>
       <c r="G4">
-        <v>5.9427993751267012</v>
+        <v>8.7719904365322421</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>3.4210526315789469</v>
       </c>
       <c r="I4">
-        <v>4.3211411142421037</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>4.41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>401</v>
+      </c>
+      <c r="K4">
+        <v>11.8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>438</v>
+      </c>
+      <c r="N4">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>113</v>
       </c>
       <c r="C5">
         <v>4.5999999999999996</v>
       </c>
       <c r="D5">
+        <v>6450</v>
+      </c>
+      <c r="E5">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G5">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H5">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I5">
+        <v>4.41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>374</v>
+      </c>
+      <c r="K5">
+        <v>11</v>
+      </c>
+      <c r="L5" t="s">
+        <v>411</v>
+      </c>
+      <c r="N5">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D6">
+        <v>6450</v>
+      </c>
+      <c r="E6">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G6">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H6">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I6">
+        <v>4.41</v>
+      </c>
+      <c r="J6" t="s">
+        <v>385</v>
+      </c>
+      <c r="K6">
+        <v>11</v>
+      </c>
+      <c r="L6" t="s">
+        <v>424</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D7">
+        <v>6450</v>
+      </c>
+      <c r="E7">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G7">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H7">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I7">
+        <v>4.41</v>
+      </c>
+      <c r="J7" t="s">
+        <v>398</v>
+      </c>
+      <c r="K7">
+        <v>10.5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>380</v>
+      </c>
+      <c r="N7">
+        <v>3.23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D8">
+        <v>6450</v>
+      </c>
+      <c r="E8">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G8">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H8">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I8">
+        <v>4.41</v>
+      </c>
+      <c r="J8" t="s">
+        <v>410</v>
+      </c>
+      <c r="K8">
+        <v>8.5</v>
+      </c>
+      <c r="L8" t="s">
+        <v>436</v>
+      </c>
+      <c r="N8">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D9">
+        <v>6450</v>
+      </c>
+      <c r="E9">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F9">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G9">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H9">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I9">
+        <v>4.41</v>
+      </c>
+      <c r="J9" t="s">
+        <v>415</v>
+      </c>
+      <c r="K9">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="L9" t="s">
+        <v>424</v>
+      </c>
+      <c r="N9">
+        <v>4.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D10">
+        <v>6450</v>
+      </c>
+      <c r="E10">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G10">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H10">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I10">
+        <v>4.41</v>
+      </c>
+      <c r="J10" t="s">
+        <v>381</v>
+      </c>
+      <c r="K10">
+        <v>6.6</v>
+      </c>
+      <c r="L10" t="s">
+        <v>436</v>
+      </c>
+      <c r="N10">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D11">
+        <v>6450</v>
+      </c>
+      <c r="E11">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F11">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G11">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H11">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I11">
+        <v>4.41</v>
+      </c>
+      <c r="J11" t="s">
+        <v>396</v>
+      </c>
+      <c r="K11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L11" t="s">
+        <v>439</v>
+      </c>
+      <c r="M11">
+        <v>88</v>
+      </c>
+      <c r="N11">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D12">
+        <v>6450</v>
+      </c>
+      <c r="E12">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G12">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H12">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I12">
+        <v>4.41</v>
+      </c>
+      <c r="J12" t="s">
+        <v>427</v>
+      </c>
+      <c r="K12">
+        <v>3.3</v>
+      </c>
+      <c r="L12" t="s">
+        <v>440</v>
+      </c>
+      <c r="M12">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D13">
+        <v>6450</v>
+      </c>
+      <c r="E13">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F13">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G13">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H13">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I13">
+        <v>4.41</v>
+      </c>
+      <c r="J13" t="s">
+        <v>409</v>
+      </c>
+      <c r="K13">
+        <v>1.2</v>
+      </c>
+      <c r="L13" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D14">
+        <v>6450</v>
+      </c>
+      <c r="E14">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G14">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H14">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I14">
+        <v>4.41</v>
+      </c>
+      <c r="J14" t="s">
+        <v>441</v>
+      </c>
+      <c r="K14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L14" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D15">
+        <v>6450</v>
+      </c>
+      <c r="E15">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F15">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G15">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H15">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I15">
+        <v>4.41</v>
+      </c>
+      <c r="J15" t="s">
+        <v>430</v>
+      </c>
+      <c r="K15">
+        <v>0.9</v>
+      </c>
+      <c r="L15" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D16">
+        <v>6450</v>
+      </c>
+      <c r="E16">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F16">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G16">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H16">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I16">
+        <v>4.41</v>
+      </c>
+      <c r="J16" t="s">
+        <v>442</v>
+      </c>
+      <c r="K16">
+        <v>0.2</v>
+      </c>
+      <c r="L16" t="s">
+        <v>443</v>
+      </c>
+      <c r="M16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D17">
+        <v>6450</v>
+      </c>
+      <c r="E17">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F17">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G17">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H17">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I17">
+        <v>4.41</v>
+      </c>
+      <c r="J17" t="s">
+        <v>444</v>
+      </c>
+      <c r="K17">
+        <v>0.2</v>
+      </c>
+      <c r="L17" t="s">
+        <v>418</v>
+      </c>
+      <c r="M17">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D18">
+        <v>6450</v>
+      </c>
+      <c r="E18">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F18">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G18">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H18">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I18">
+        <v>4.41</v>
+      </c>
+      <c r="J18" t="s">
+        <v>445</v>
+      </c>
+      <c r="K18">
+        <v>0.1</v>
+      </c>
+      <c r="L18" t="s">
+        <v>421</v>
+      </c>
+      <c r="M18">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D19">
+        <v>6450</v>
+      </c>
+      <c r="E19">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F19">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G19">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H19">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I19">
+        <v>4.41</v>
+      </c>
+      <c r="J19" t="s">
+        <v>446</v>
+      </c>
+      <c r="K19">
+        <v>0.1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D20">
+        <v>6450</v>
+      </c>
+      <c r="E20">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="F20">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="G20">
+        <v>8.7719904365322421</v>
+      </c>
+      <c r="H20">
+        <v>3.4210526315789469</v>
+      </c>
+      <c r="I20">
+        <v>4.41</v>
+      </c>
+      <c r="J20" t="s">
+        <v>447</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>310</v>
+      </c>
+      <c r="B21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C21">
+        <v>4.7</v>
+      </c>
+      <c r="D21">
+        <v>627</v>
+      </c>
+      <c r="E21">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F21">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G21">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H21">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I21">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J21" t="s">
+        <v>387</v>
+      </c>
+      <c r="K21">
+        <v>22.3</v>
+      </c>
+      <c r="L21" t="s">
+        <v>437</v>
+      </c>
+      <c r="N21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>310</v>
+      </c>
+      <c r="B22" t="s">
+        <v>311</v>
+      </c>
+      <c r="C22">
+        <v>4.7</v>
+      </c>
+      <c r="D22">
+        <v>627</v>
+      </c>
+      <c r="E22">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F22">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G22">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H22">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I22">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J22" t="s">
+        <v>372</v>
+      </c>
+      <c r="K22">
+        <v>18</v>
+      </c>
+      <c r="L22" t="s">
+        <v>408</v>
+      </c>
+      <c r="N22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>310</v>
+      </c>
+      <c r="B23" t="s">
+        <v>311</v>
+      </c>
+      <c r="C23">
+        <v>4.7</v>
+      </c>
+      <c r="D23">
+        <v>627</v>
+      </c>
+      <c r="E23">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F23">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G23">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H23">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I23">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J23" t="s">
+        <v>401</v>
+      </c>
+      <c r="K23">
+        <v>14.5</v>
+      </c>
+      <c r="L23" t="s">
+        <v>388</v>
+      </c>
+      <c r="N23">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>310</v>
+      </c>
+      <c r="B24" t="s">
+        <v>311</v>
+      </c>
+      <c r="C24">
+        <v>4.7</v>
+      </c>
+      <c r="D24">
+        <v>627</v>
+      </c>
+      <c r="E24">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F24">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G24">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H24">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I24">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J24" t="s">
+        <v>370</v>
+      </c>
+      <c r="K24">
+        <v>12.9</v>
+      </c>
+      <c r="L24" t="s">
+        <v>384</v>
+      </c>
+      <c r="N24">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>310</v>
+      </c>
+      <c r="B25" t="s">
+        <v>311</v>
+      </c>
+      <c r="C25">
+        <v>4.7</v>
+      </c>
+      <c r="D25">
+        <v>627</v>
+      </c>
+      <c r="E25">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F25">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G25">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H25">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I25">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J25" t="s">
+        <v>385</v>
+      </c>
+      <c r="K25">
+        <v>12</v>
+      </c>
+      <c r="L25" t="s">
+        <v>405</v>
+      </c>
+      <c r="N25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>310</v>
+      </c>
+      <c r="B26" t="s">
+        <v>311</v>
+      </c>
+      <c r="C26">
+        <v>4.7</v>
+      </c>
+      <c r="D26">
+        <v>627</v>
+      </c>
+      <c r="E26">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F26">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G26">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H26">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I26">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J26" t="s">
+        <v>381</v>
+      </c>
+      <c r="K26">
+        <v>7.7</v>
+      </c>
+      <c r="L26" t="s">
+        <v>406</v>
+      </c>
+      <c r="N26">
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B27" t="s">
+        <v>311</v>
+      </c>
+      <c r="C27">
+        <v>4.7</v>
+      </c>
+      <c r="D27">
+        <v>627</v>
+      </c>
+      <c r="E27">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F27">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G27">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H27">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I27">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J27" t="s">
+        <v>374</v>
+      </c>
+      <c r="K27">
+        <v>8.6</v>
+      </c>
+      <c r="L27" t="s">
+        <v>429</v>
+      </c>
+      <c r="N27">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>310</v>
+      </c>
+      <c r="B28" t="s">
+        <v>311</v>
+      </c>
+      <c r="C28">
+        <v>4.7</v>
+      </c>
+      <c r="D28">
+        <v>627</v>
+      </c>
+      <c r="E28">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F28">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G28">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H28">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I28">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J28" t="s">
+        <v>410</v>
+      </c>
+      <c r="K28">
+        <v>6.4</v>
+      </c>
+      <c r="L28" t="s">
+        <v>429</v>
+      </c>
+      <c r="N28">
+        <v>4.82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>310</v>
+      </c>
+      <c r="B29" t="s">
+        <v>311</v>
+      </c>
+      <c r="C29">
+        <v>4.7</v>
+      </c>
+      <c r="D29">
+        <v>627</v>
+      </c>
+      <c r="E29">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F29">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G29">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H29">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I29">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J29" t="s">
+        <v>480</v>
+      </c>
+      <c r="K29">
+        <v>6.4</v>
+      </c>
+      <c r="L29" t="s">
+        <v>422</v>
+      </c>
+      <c r="N29">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>310</v>
+      </c>
+      <c r="B30" t="s">
+        <v>311</v>
+      </c>
+      <c r="C30">
+        <v>4.7</v>
+      </c>
+      <c r="D30">
+        <v>627</v>
+      </c>
+      <c r="E30">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F30">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G30">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H30">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I30">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J30" t="s">
+        <v>415</v>
+      </c>
+      <c r="K30">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L30" t="s">
+        <v>456</v>
+      </c>
+      <c r="N30">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>310</v>
+      </c>
+      <c r="B31" t="s">
+        <v>311</v>
+      </c>
+      <c r="C31">
+        <v>4.7</v>
+      </c>
+      <c r="D31">
+        <v>627</v>
+      </c>
+      <c r="E31">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F31">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G31">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H31">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I31">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J31" t="s">
+        <v>403</v>
+      </c>
+      <c r="K31">
+        <v>3</v>
+      </c>
+      <c r="L31" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>310</v>
+      </c>
+      <c r="B32" t="s">
+        <v>311</v>
+      </c>
+      <c r="C32">
+        <v>4.7</v>
+      </c>
+      <c r="D32">
+        <v>627</v>
+      </c>
+      <c r="E32">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F32">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G32">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H32">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I32">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J32" t="s">
+        <v>430</v>
+      </c>
+      <c r="K32">
+        <v>1.6</v>
+      </c>
+      <c r="L32" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>310</v>
+      </c>
+      <c r="B33" t="s">
+        <v>311</v>
+      </c>
+      <c r="C33">
+        <v>4.7</v>
+      </c>
+      <c r="D33">
+        <v>627</v>
+      </c>
+      <c r="E33">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F33">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G33">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H33">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I33">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J33" t="s">
+        <v>390</v>
+      </c>
+      <c r="K33">
+        <v>1.3</v>
+      </c>
+      <c r="L33" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>310</v>
+      </c>
+      <c r="B34" t="s">
+        <v>311</v>
+      </c>
+      <c r="C34">
+        <v>4.7</v>
+      </c>
+      <c r="D34">
+        <v>627</v>
+      </c>
+      <c r="E34">
+        <v>4.5579999999999998</v>
+      </c>
+      <c r="F34">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G34">
+        <v>6.4425401664681976</v>
+      </c>
+      <c r="H34">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="I34">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J34" t="s">
+        <v>481</v>
+      </c>
+      <c r="K34">
+        <v>0.2</v>
+      </c>
+      <c r="L34" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35">
+        <v>4.5</v>
+      </c>
+      <c r="D35">
+        <v>1143</v>
+      </c>
+      <c r="E35">
+        <v>4.5062499999999996</v>
+      </c>
+      <c r="F35">
+        <v>0.6</v>
+      </c>
+      <c r="G35">
+        <v>7.0422861719397432</v>
+      </c>
+      <c r="H35">
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <v>4.26</v>
+      </c>
+      <c r="J35" t="s">
+        <v>385</v>
+      </c>
+      <c r="K35">
+        <v>18.5</v>
+      </c>
+      <c r="L35" t="s">
+        <v>424</v>
+      </c>
+      <c r="N35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36">
+        <v>4.5</v>
+      </c>
+      <c r="D36">
+        <v>1143</v>
+      </c>
+      <c r="E36">
+        <v>4.5062499999999996</v>
+      </c>
+      <c r="F36">
+        <v>0.6</v>
+      </c>
+      <c r="G36">
+        <v>7.0422861719397432</v>
+      </c>
+      <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="I36">
+        <v>4.26</v>
+      </c>
+      <c r="J36" t="s">
+        <v>372</v>
+      </c>
+      <c r="K36">
+        <v>14.9</v>
+      </c>
+      <c r="L36" t="s">
+        <v>408</v>
+      </c>
+      <c r="N36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37">
+        <v>4.5</v>
+      </c>
+      <c r="D37">
+        <v>1143</v>
+      </c>
+      <c r="E37">
+        <v>4.5062499999999996</v>
+      </c>
+      <c r="F37">
+        <v>0.6</v>
+      </c>
+      <c r="G37">
+        <v>7.0422861719397432</v>
+      </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+      <c r="I37">
+        <v>4.26</v>
+      </c>
+      <c r="J37" t="s">
+        <v>415</v>
+      </c>
+      <c r="K37">
+        <v>12.8</v>
+      </c>
+      <c r="L37" t="s">
+        <v>406</v>
+      </c>
+      <c r="N37">
+        <v>4.46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38">
+        <v>4.5</v>
+      </c>
+      <c r="D38">
+        <v>1143</v>
+      </c>
+      <c r="E38">
+        <v>4.5062499999999996</v>
+      </c>
+      <c r="F38">
+        <v>0.6</v>
+      </c>
+      <c r="G38">
+        <v>7.0422861719397432</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+      <c r="I38">
+        <v>4.26</v>
+      </c>
+      <c r="J38" t="s">
+        <v>370</v>
+      </c>
+      <c r="K38">
+        <v>10.1</v>
+      </c>
+      <c r="L38" t="s">
+        <v>432</v>
+      </c>
+      <c r="N38">
+        <v>4.1900000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39">
+        <v>4.5</v>
+      </c>
+      <c r="D39">
+        <v>1143</v>
+      </c>
+      <c r="E39">
+        <v>4.5062499999999996</v>
+      </c>
+      <c r="F39">
+        <v>0.6</v>
+      </c>
+      <c r="G39">
+        <v>7.0422861719397432</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+      <c r="I39">
+        <v>4.26</v>
+      </c>
+      <c r="J39" t="s">
+        <v>381</v>
+      </c>
+      <c r="K39">
+        <v>11</v>
+      </c>
+      <c r="L39" t="s">
+        <v>433</v>
+      </c>
+      <c r="N39">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40">
+        <v>4.5</v>
+      </c>
+      <c r="D40">
+        <v>1143</v>
+      </c>
+      <c r="E40">
+        <v>4.5062499999999996</v>
+      </c>
+      <c r="F40">
+        <v>0.6</v>
+      </c>
+      <c r="G40">
+        <v>7.0422861719397432</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>4.26</v>
+      </c>
+      <c r="J40" t="s">
+        <v>410</v>
+      </c>
+      <c r="K40">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="L40" t="s">
+        <v>431</v>
+      </c>
+      <c r="N40">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41">
+        <v>4.5</v>
+      </c>
+      <c r="D41">
+        <v>1143</v>
+      </c>
+      <c r="E41">
+        <v>4.5062499999999996</v>
+      </c>
+      <c r="F41">
+        <v>0.6</v>
+      </c>
+      <c r="G41">
+        <v>7.0422861719397432</v>
+      </c>
+      <c r="H41">
+        <v>3</v>
+      </c>
+      <c r="I41">
+        <v>4.26</v>
+      </c>
+      <c r="J41" t="s">
+        <v>403</v>
+      </c>
+      <c r="K41">
+        <v>7.6</v>
+      </c>
+      <c r="L41" t="s">
+        <v>434</v>
+      </c>
+      <c r="N41">
+        <v>3.23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42">
+        <v>4.5</v>
+      </c>
+      <c r="D42">
+        <v>1143</v>
+      </c>
+      <c r="E42">
+        <v>4.5062499999999996</v>
+      </c>
+      <c r="F42">
+        <v>0.6</v>
+      </c>
+      <c r="G42">
+        <v>7.0422861719397432</v>
+      </c>
+      <c r="H42">
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <v>4.26</v>
+      </c>
+      <c r="J42" t="s">
+        <v>387</v>
+      </c>
+      <c r="K42">
+        <v>4.7</v>
+      </c>
+      <c r="L42" t="s">
+        <v>429</v>
+      </c>
+      <c r="N42">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43">
+        <v>4.5</v>
+      </c>
+      <c r="D43">
+        <v>1143</v>
+      </c>
+      <c r="E43">
+        <v>4.5062499999999996</v>
+      </c>
+      <c r="F43">
+        <v>0.6</v>
+      </c>
+      <c r="G43">
+        <v>7.0422861719397432</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+      <c r="I43">
+        <v>4.26</v>
+      </c>
+      <c r="J43" t="s">
+        <v>409</v>
+      </c>
+      <c r="K43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L43" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44">
+        <v>4.5</v>
+      </c>
+      <c r="D44">
+        <v>1143</v>
+      </c>
+      <c r="E44">
+        <v>4.5062499999999996</v>
+      </c>
+      <c r="F44">
+        <v>0.6</v>
+      </c>
+      <c r="G44">
+        <v>7.0422861719397432</v>
+      </c>
+      <c r="H44">
+        <v>3</v>
+      </c>
+      <c r="I44">
+        <v>4.26</v>
+      </c>
+      <c r="J44" t="s">
+        <v>392</v>
+      </c>
+      <c r="K44">
+        <v>0.8</v>
+      </c>
+      <c r="L44" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D45">
         <v>317</v>
       </c>
-      <c r="E5">
+      <c r="E45">
         <v>4.5055555555555564</v>
       </c>
-      <c r="F5">
+      <c r="F45">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G5">
+      <c r="G45">
         <v>5.7620513827801769</v>
       </c>
-      <c r="H5">
+      <c r="H45">
         <v>4.166666666666667</v>
       </c>
-      <c r="I5">
-        <v>4.221869318824524</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="I45">
+        <v>4.26</v>
+      </c>
+      <c r="J45" t="s">
+        <v>370</v>
+      </c>
+      <c r="K45">
+        <v>24.9</v>
+      </c>
+      <c r="L45" t="s">
+        <v>456</v>
+      </c>
+      <c r="N45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D46">
+        <v>317</v>
+      </c>
+      <c r="E46">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F46">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G46">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H46">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I46">
+        <v>4.26</v>
+      </c>
+      <c r="J46" t="s">
+        <v>372</v>
+      </c>
+      <c r="K46">
+        <v>20.8</v>
+      </c>
+      <c r="L46" t="s">
+        <v>431</v>
+      </c>
+      <c r="N46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>172</v>
+      </c>
+      <c r="B47" t="s">
+        <v>173</v>
+      </c>
+      <c r="C47">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D47">
+        <v>317</v>
+      </c>
+      <c r="E47">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F47">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G47">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H47">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I47">
+        <v>4.26</v>
+      </c>
+      <c r="J47" t="s">
+        <v>374</v>
+      </c>
+      <c r="K47">
+        <v>13.9</v>
+      </c>
+      <c r="L47" t="s">
+        <v>457</v>
+      </c>
+      <c r="N47">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>172</v>
+      </c>
+      <c r="B48" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D48">
+        <v>317</v>
+      </c>
+      <c r="E48">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F48">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G48">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H48">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I48">
+        <v>4.26</v>
+      </c>
+      <c r="J48" t="s">
+        <v>376</v>
+      </c>
+      <c r="K48">
+        <v>14.8</v>
+      </c>
+      <c r="L48" t="s">
+        <v>408</v>
+      </c>
+      <c r="N48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>172</v>
+      </c>
+      <c r="B49" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D49">
+        <v>317</v>
+      </c>
+      <c r="E49">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F49">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G49">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H49">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I49">
+        <v>4.26</v>
+      </c>
+      <c r="J49" t="s">
+        <v>415</v>
+      </c>
+      <c r="K49">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L49" t="s">
+        <v>451</v>
+      </c>
+      <c r="N49">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D50">
+        <v>317</v>
+      </c>
+      <c r="E50">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F50">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G50">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H50">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I50">
+        <v>4.26</v>
+      </c>
+      <c r="J50" t="s">
+        <v>381</v>
+      </c>
+      <c r="K50">
+        <v>10.1</v>
+      </c>
+      <c r="L50" t="s">
+        <v>456</v>
+      </c>
+      <c r="N50">
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>172</v>
+      </c>
+      <c r="B51" t="s">
+        <v>173</v>
+      </c>
+      <c r="C51">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D51">
+        <v>317</v>
+      </c>
+      <c r="E51">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F51">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G51">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H51">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I51">
+        <v>4.26</v>
+      </c>
+      <c r="J51" t="s">
+        <v>383</v>
+      </c>
+      <c r="K51">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L51" t="s">
+        <v>405</v>
+      </c>
+      <c r="N51">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" t="s">
+        <v>173</v>
+      </c>
+      <c r="C52">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D52">
+        <v>317</v>
+      </c>
+      <c r="E52">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F52">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G52">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H52">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I52">
+        <v>4.26</v>
+      </c>
+      <c r="J52" t="s">
+        <v>377</v>
+      </c>
+      <c r="K52">
+        <v>7.9</v>
+      </c>
+      <c r="L52" t="s">
+        <v>458</v>
+      </c>
+      <c r="N52">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>172</v>
+      </c>
+      <c r="B53" t="s">
+        <v>173</v>
+      </c>
+      <c r="C53">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D53">
+        <v>317</v>
+      </c>
+      <c r="E53">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F53">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G53">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H53">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I53">
+        <v>4.26</v>
+      </c>
+      <c r="J53" t="s">
+        <v>385</v>
+      </c>
+      <c r="K53">
+        <v>5.7</v>
+      </c>
+      <c r="L53" t="s">
+        <v>371</v>
+      </c>
+      <c r="N53">
+        <v>4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>172</v>
+      </c>
+      <c r="B54" t="s">
+        <v>173</v>
+      </c>
+      <c r="C54">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D54">
+        <v>317</v>
+      </c>
+      <c r="E54">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F54">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G54">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H54">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I54">
+        <v>4.26</v>
+      </c>
+      <c r="J54" t="s">
+        <v>459</v>
+      </c>
+      <c r="K54">
+        <v>2.8</v>
+      </c>
+      <c r="L54" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" t="s">
+        <v>173</v>
+      </c>
+      <c r="C55">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D55">
+        <v>317</v>
+      </c>
+      <c r="E55">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F55">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G55">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H55">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I55">
+        <v>4.26</v>
+      </c>
+      <c r="J55" t="s">
+        <v>389</v>
+      </c>
+      <c r="K55">
+        <v>1.9</v>
+      </c>
+      <c r="L55" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B56" t="s">
+        <v>173</v>
+      </c>
+      <c r="C56">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D56">
+        <v>317</v>
+      </c>
+      <c r="E56">
+        <v>4.5055555555555564</v>
+      </c>
+      <c r="F56">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G56">
+        <v>5.7620513827801769</v>
+      </c>
+      <c r="H56">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I56">
+        <v>4.26</v>
+      </c>
+      <c r="J56" t="s">
+        <v>390</v>
+      </c>
+      <c r="K56">
+        <v>0.3</v>
+      </c>
+      <c r="L56" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>329</v>
+      </c>
+      <c r="B57" t="s">
+        <v>330</v>
+      </c>
+      <c r="C57">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D57">
+        <v>380</v>
+      </c>
+      <c r="E57">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H57">
+        <v>5</v>
+      </c>
+      <c r="I57">
+        <v>4.24</v>
+      </c>
+      <c r="J57" t="s">
+        <v>374</v>
+      </c>
+      <c r="K57">
+        <v>28.4</v>
+      </c>
+      <c r="L57" t="s">
+        <v>482</v>
+      </c>
+      <c r="N57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>329</v>
+      </c>
+      <c r="B58" t="s">
+        <v>330</v>
+      </c>
+      <c r="C58">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D58">
+        <v>380</v>
+      </c>
+      <c r="E58">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H58">
+        <v>5</v>
+      </c>
+      <c r="I58">
+        <v>4.24</v>
+      </c>
+      <c r="J58" t="s">
+        <v>415</v>
+      </c>
+      <c r="K58">
+        <v>31.6</v>
+      </c>
+      <c r="L58" t="s">
+        <v>419</v>
+      </c>
+      <c r="N58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>329</v>
+      </c>
+      <c r="B59" t="s">
+        <v>330</v>
+      </c>
+      <c r="C59">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D59">
+        <v>380</v>
+      </c>
+      <c r="E59">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H59">
+        <v>5</v>
+      </c>
+      <c r="I59">
+        <v>4.24</v>
+      </c>
+      <c r="J59" t="s">
+        <v>381</v>
+      </c>
+      <c r="K59">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="L59" t="s">
+        <v>419</v>
+      </c>
+      <c r="N59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>329</v>
+      </c>
+      <c r="B60" t="s">
+        <v>330</v>
+      </c>
+      <c r="C60">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D60">
+        <v>380</v>
+      </c>
+      <c r="E60">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H60">
+        <v>5</v>
+      </c>
+      <c r="I60">
+        <v>4.24</v>
+      </c>
+      <c r="J60" t="s">
+        <v>398</v>
+      </c>
+      <c r="K60">
+        <v>18.7</v>
+      </c>
+      <c r="L60" t="s">
+        <v>395</v>
+      </c>
+      <c r="N60">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>329</v>
+      </c>
+      <c r="B61" t="s">
+        <v>330</v>
+      </c>
+      <c r="C61">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D61">
+        <v>380</v>
+      </c>
+      <c r="E61">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H61">
+        <v>5</v>
+      </c>
+      <c r="I61">
+        <v>4.24</v>
+      </c>
+      <c r="J61" t="s">
+        <v>401</v>
+      </c>
+      <c r="K61">
+        <v>7.6</v>
+      </c>
+      <c r="L61" t="s">
+        <v>453</v>
+      </c>
+      <c r="N61">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>329</v>
+      </c>
+      <c r="B62" t="s">
+        <v>330</v>
+      </c>
+      <c r="C62">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D62">
+        <v>380</v>
+      </c>
+      <c r="E62">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H62">
+        <v>5</v>
+      </c>
+      <c r="I62">
+        <v>4.24</v>
+      </c>
+      <c r="J62" t="s">
+        <v>385</v>
+      </c>
+      <c r="K62">
+        <v>7.4</v>
+      </c>
+      <c r="L62" t="s">
+        <v>431</v>
+      </c>
+      <c r="N62">
+        <v>4.5199999999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>329</v>
+      </c>
+      <c r="B63" t="s">
+        <v>330</v>
+      </c>
+      <c r="C63">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D63">
+        <v>380</v>
+      </c>
+      <c r="E63">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H63">
+        <v>5</v>
+      </c>
+      <c r="I63">
+        <v>4.24</v>
+      </c>
+      <c r="J63" t="s">
+        <v>480</v>
+      </c>
+      <c r="K63">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L63" t="s">
+        <v>464</v>
+      </c>
+      <c r="M63">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D6">
-        <v>461</v>
-      </c>
-      <c r="E6">
-        <v>3.78</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>6.1355648910817386</v>
-      </c>
-      <c r="H6">
+      <c r="N63">
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>329</v>
+      </c>
+      <c r="B64" t="s">
+        <v>330</v>
+      </c>
+      <c r="C64">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D64">
+        <v>380</v>
+      </c>
+      <c r="E64">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H64">
         <v>5</v>
       </c>
-      <c r="I6">
-        <v>4.1534495645514236</v>
+      <c r="I64">
+        <v>4.24</v>
+      </c>
+      <c r="J64" t="s">
+        <v>383</v>
+      </c>
+      <c r="K64">
+        <v>5.5</v>
+      </c>
+      <c r="L64" t="s">
+        <v>402</v>
+      </c>
+      <c r="N64">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>329</v>
+      </c>
+      <c r="B65" t="s">
+        <v>330</v>
+      </c>
+      <c r="C65">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D65">
+        <v>380</v>
+      </c>
+      <c r="E65">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H65">
+        <v>5</v>
+      </c>
+      <c r="I65">
+        <v>4.24</v>
+      </c>
+      <c r="J65" t="s">
+        <v>387</v>
+      </c>
+      <c r="K65">
+        <v>7.1</v>
+      </c>
+      <c r="L65" t="s">
+        <v>405</v>
+      </c>
+      <c r="N65">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>329</v>
+      </c>
+      <c r="B66" t="s">
+        <v>330</v>
+      </c>
+      <c r="C66">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D66">
+        <v>380</v>
+      </c>
+      <c r="E66">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H66">
+        <v>5</v>
+      </c>
+      <c r="I66">
+        <v>4.24</v>
+      </c>
+      <c r="J66" t="s">
+        <v>392</v>
+      </c>
+      <c r="K66">
+        <v>2.6</v>
+      </c>
+      <c r="L66" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>329</v>
+      </c>
+      <c r="B67" t="s">
+        <v>330</v>
+      </c>
+      <c r="C67">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D67">
+        <v>380</v>
+      </c>
+      <c r="E67">
+        <v>4.2122222222222216</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>5.9427993751267012</v>
+      </c>
+      <c r="H67">
+        <v>5</v>
+      </c>
+      <c r="I67">
+        <v>4.24</v>
+      </c>
+      <c r="J67" t="s">
+        <v>390</v>
+      </c>
+      <c r="K67">
+        <v>2.4</v>
+      </c>
+      <c r="L67" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>